<commit_message>
separate P1 P3, export motorbike, remain  exportModal bug on motor, close tour rental
</commit_message>
<xml_diff>
--- a/static/templates/motorbike_agreement_template.xlsx
+++ b/static/templates/motorbike_agreement_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00.Work_Freelance\Tour\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F660497A-E122-43C5-A94D-21E6615AE337}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ACEEB0-F7A4-40A6-92A5-B865B2B53F90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8865" xr2:uid="{492F029A-8E98-4A79-9B77-CF9AB15A96C9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8868" xr2:uid="{492F029A-8E98-4A79-9B77-CF9AB15A96C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>LAMAI BAYVIEW BOUTIQUE RESORT</t>
   </si>
@@ -701,24 +701,12 @@
     <t>No.</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Travel date</t>
-  </si>
-  <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>Room</t>
-  </si>
-  <si>
     <t>ROOM NO.</t>
   </si>
   <si>
-    <t>Name&amp;Surmane</t>
-  </si>
-  <si>
     <t>TEL : +66 77 420 789    E-MAIL : info@lamaibayviewboutique.co.th</t>
   </si>
   <si>
@@ -728,15 +716,9 @@
     <t>Lamai Bayview Boutique Resort</t>
   </si>
   <si>
-    <t>Booking No.</t>
-  </si>
-  <si>
     <t>BOOKING NO.</t>
   </si>
   <si>
-    <t>Booking date</t>
-  </si>
-  <si>
     <t>BOOKING CONFIRMATION</t>
   </si>
   <si>
@@ -744,12 +726,6 @@
   </si>
   <si>
     <t>Price / Quantity</t>
-  </si>
-  <si>
-    <t>Remark</t>
-  </si>
-  <si>
-    <t>Payment</t>
   </si>
   <si>
     <t xml:space="preserve">                 BOOKING NO. </t>
@@ -1098,46 +1074,46 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1457,30 +1433,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F97E37-B014-4C99-B27C-6BC54D2AD0E2}">
   <dimension ref="A1:AG59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="P1" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="2.5" style="7" customWidth="1"/>
     <col min="2" max="6" width="9" style="7"/>
     <col min="7" max="7" width="6.5" style="7" customWidth="1"/>
-    <col min="8" max="8" width="8.375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="9.125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="8.3984375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="9.09765625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" style="7" customWidth="1"/>
     <col min="11" max="11" width="1.5" style="8" customWidth="1"/>
     <col min="12" max="12" width="2.5" style="1" customWidth="1"/>
     <col min="13" max="17" width="9" style="1"/>
     <col min="18" max="18" width="6.5" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="1"/>
     <col min="21" max="21" width="7.5" style="1" customWidth="1"/>
     <col min="22" max="22" width="1.5" style="1" customWidth="1"/>
     <col min="23" max="23" width="2.5" style="1" customWidth="1"/>
     <col min="24" max="28" width="9" style="1"/>
     <col min="29" max="29" width="6.5" style="1" customWidth="1"/>
-    <col min="30" max="30" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" style="1"/>
     <col min="32" max="32" width="7.5" style="1" customWidth="1"/>
     <col min="33" max="33" width="1.5" style="1" customWidth="1"/>
@@ -1489,22 +1465,22 @@
   <sheetData>
     <row r="1" spans="1:33" ht="8.25" customHeight="1"/>
     <row r="2" spans="1:33" ht="21" customHeight="1">
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="T2" s="51" t="s">
+      <c r="J2" s="38"/>
+      <c r="T2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="51"/>
-      <c r="AE2" s="51" t="s">
+      <c r="U2" s="41"/>
+      <c r="AE2" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="AF2" s="51"/>
+      <c r="AF2" s="41"/>
     </row>
     <row r="3" spans="1:33" ht="12" customHeight="1">
       <c r="D3" s="45" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="45"/>
       <c r="F3" s="45"/>
@@ -1518,37 +1494,34 @@
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
-      <c r="I4" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
-      <c r="L4" s="40" t="s">
+      <c r="L4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="40" t="s">
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="40"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="42"/>
+      <c r="AG4" s="42"/>
     </row>
     <row r="5" spans="1:33" ht="3.75" customHeight="1"/>
     <row r="6" spans="1:33">
@@ -1558,77 +1531,74 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="G6" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="51"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="41" t="s">
+      <c r="L6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41" t="s">
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="41"/>
-      <c r="AE6" s="41"/>
-      <c r="AF6" s="41"/>
-      <c r="AG6" s="41"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="43"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="43"/>
+      <c r="AF6" s="43"/>
+      <c r="AG6" s="43"/>
     </row>
     <row r="7" spans="1:33" ht="17.25" customHeight="1">
       <c r="B7" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K7" s="7"/>
-      <c r="L7" s="47" t="s">
+      <c r="L7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="47"/>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="47" t="s">
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="44"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="X7" s="47"/>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="47"/>
-      <c r="AA7" s="47"/>
-      <c r="AB7" s="47"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="47"/>
-      <c r="AE7" s="47"/>
-      <c r="AF7" s="47"/>
-      <c r="AG7" s="47"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44"/>
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="44"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="44"/>
+      <c r="AF7" s="44"/>
+      <c r="AG7" s="44"/>
     </row>
     <row r="8" spans="1:33" ht="15.75" customHeight="1">
       <c r="B8" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1639,37 +1609,37 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="47" t="s">
+      <c r="L8" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47" t="s">
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="47"/>
-      <c r="Z8" s="47"/>
-      <c r="AA8" s="47"/>
-      <c r="AB8" s="47"/>
-      <c r="AC8" s="47"/>
-      <c r="AD8" s="47"/>
-      <c r="AE8" s="47"/>
-      <c r="AF8" s="47"/>
-      <c r="AG8" s="47"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="44"/>
+      <c r="Z8" s="44"/>
+      <c r="AA8" s="44"/>
+      <c r="AB8" s="44"/>
+      <c r="AC8" s="44"/>
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="44"/>
+      <c r="AF8" s="44"/>
+      <c r="AG8" s="44"/>
     </row>
     <row r="9" spans="1:33" ht="14.25" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1707,7 +1677,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="T10" s="9"/>
       <c r="U10" s="4"/>
@@ -1718,7 +1688,7 @@
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
       <c r="AC10" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AE10" s="9"/>
       <c r="AF10" s="4"/>
@@ -1727,9 +1697,6 @@
       <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="M11" s="10" t="s">
         <v>5</v>
       </c>
@@ -1745,29 +1712,18 @@
     </row>
     <row r="12" spans="1:33">
       <c r="B12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="M12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N12" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="N12" s="9"/>
       <c r="R12" s="9" t="s">
         <v>9</v>
       </c>
@@ -1779,9 +1735,7 @@
       <c r="X12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="Y12" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="Y12" s="9"/>
       <c r="AC12" s="9" t="s">
         <v>9</v>
       </c>
@@ -1789,7 +1743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" ht="15">
       <c r="B13" s="14" t="s">
         <v>31</v>
       </c>
@@ -1799,10 +1753,10 @@
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="44"/>
+      <c r="G13" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="47"/>
       <c r="I13" s="19" t="s">
         <v>29</v>
       </c>
@@ -1812,15 +1766,11 @@
       <c r="M13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="N13" s="9"/>
       <c r="O13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P13" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="P13" s="9"/>
       <c r="R13" s="9" t="s">
         <v>10</v>
       </c>
@@ -1831,15 +1781,11 @@
       <c r="X13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Y13" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="Y13" s="9"/>
       <c r="Z13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AA13" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="AA13" s="9"/>
       <c r="AC13" s="9" t="s">
         <v>10</v>
       </c>
@@ -1848,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" ht="15">
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17"/>
@@ -1861,15 +1807,11 @@
       <c r="M14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N14" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="N14" s="9"/>
       <c r="O14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P14" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="P14" s="9"/>
       <c r="R14" s="9" t="s">
         <v>12</v>
       </c>
@@ -1879,15 +1821,11 @@
       <c r="X14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Y14" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="Y14" s="9"/>
       <c r="Z14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AA14" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="AA14" s="9"/>
       <c r="AC14" s="9" t="s">
         <v>12</v>
       </c>
@@ -1895,7 +1833,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" ht="15">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
@@ -1910,7 +1848,7 @@
       <c r="X15" s="9"/>
       <c r="AC15" s="9"/>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" ht="15">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
@@ -1929,7 +1867,7 @@
       </c>
       <c r="AC16" s="9"/>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" ht="15">
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
@@ -1948,7 +1886,7 @@
       </c>
       <c r="AC17" s="9"/>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" ht="15">
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
@@ -1964,128 +1902,122 @@
       <c r="AC18" s="9"/>
     </row>
     <row r="19" spans="1:32" ht="14.25" customHeight="1">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="39"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
       <c r="J19" s="32"/>
-      <c r="M19" s="50" t="s">
+      <c r="M19" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="50"/>
-      <c r="S19" s="50"/>
-      <c r="T19" s="50"/>
-      <c r="U19" s="50"/>
-      <c r="X19" s="50" t="s">
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="X19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="Y19" s="50"/>
-      <c r="Z19" s="50"/>
-      <c r="AA19" s="50"/>
-      <c r="AB19" s="50"/>
-      <c r="AC19" s="50"/>
-      <c r="AD19" s="50"/>
-      <c r="AE19" s="50"/>
-      <c r="AF19" s="50"/>
-    </row>
-    <row r="20" spans="1:32">
+      <c r="Y19" s="40"/>
+      <c r="Z19" s="40"/>
+      <c r="AA19" s="40"/>
+      <c r="AB19" s="40"/>
+      <c r="AC19" s="40"/>
+      <c r="AD19" s="40"/>
+      <c r="AE19" s="40"/>
+      <c r="AF19" s="40"/>
+    </row>
+    <row r="20" spans="1:32" ht="15">
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="39"/>
+      <c r="I20" s="50"/>
       <c r="J20" s="33">
         <f>SUM(J14:J19)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="50"/>
-      <c r="S20" s="50"/>
-      <c r="T20" s="50"/>
-      <c r="U20" s="50"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="50"/>
-      <c r="Z20" s="50"/>
-      <c r="AA20" s="50"/>
-      <c r="AB20" s="50"/>
-      <c r="AC20" s="50"/>
-      <c r="AD20" s="50"/>
-      <c r="AE20" s="50"/>
-      <c r="AF20" s="50"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="40"/>
+      <c r="AA20" s="40"/>
+      <c r="AB20" s="40"/>
+      <c r="AC20" s="40"/>
+      <c r="AD20" s="40"/>
+      <c r="AE20" s="40"/>
+      <c r="AF20" s="40"/>
     </row>
     <row r="21" spans="1:32">
       <c r="B21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="50"/>
-      <c r="T21" s="50"/>
-      <c r="U21" s="50"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="50"/>
-      <c r="AB21" s="50"/>
-      <c r="AC21" s="50"/>
-      <c r="AD21" s="50"/>
-      <c r="AE21" s="50"/>
-      <c r="AF21" s="50"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="X21" s="40"/>
+      <c r="Y21" s="40"/>
+      <c r="Z21" s="40"/>
+      <c r="AA21" s="40"/>
+      <c r="AB21" s="40"/>
+      <c r="AC21" s="40"/>
+      <c r="AD21" s="40"/>
+      <c r="AE21" s="40"/>
+      <c r="AF21" s="40"/>
     </row>
     <row r="22" spans="1:32">
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="50"/>
-      <c r="R22" s="50"/>
-      <c r="S22" s="50"/>
-      <c r="T22" s="50"/>
-      <c r="U22" s="50"/>
-      <c r="X22" s="50"/>
-      <c r="Y22" s="50"/>
-      <c r="Z22" s="50"/>
-      <c r="AA22" s="50"/>
-      <c r="AB22" s="50"/>
-      <c r="AC22" s="50"/>
-      <c r="AD22" s="50"/>
-      <c r="AE22" s="50"/>
-      <c r="AF22" s="50"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="X22" s="40"/>
+      <c r="Y22" s="40"/>
+      <c r="Z22" s="40"/>
+      <c r="AA22" s="40"/>
+      <c r="AB22" s="40"/>
+      <c r="AC22" s="40"/>
+      <c r="AD22" s="40"/>
+      <c r="AE22" s="40"/>
+      <c r="AF22" s="40"/>
     </row>
     <row r="23" spans="1:32">
       <c r="B23" s="24"/>
@@ -2099,44 +2031,44 @@
       <c r="J23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="50"/>
-      <c r="T23" s="50"/>
-      <c r="U23" s="50"/>
-      <c r="X23" s="50"/>
-      <c r="Y23" s="50"/>
-      <c r="Z23" s="50"/>
-      <c r="AA23" s="50"/>
-      <c r="AB23" s="50"/>
-      <c r="AC23" s="50"/>
-      <c r="AD23" s="50"/>
-      <c r="AE23" s="50"/>
-      <c r="AF23" s="50"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="40"/>
+      <c r="AA23" s="40"/>
+      <c r="AB23" s="40"/>
+      <c r="AC23" s="40"/>
+      <c r="AD23" s="40"/>
+      <c r="AE23" s="40"/>
+      <c r="AF23" s="40"/>
     </row>
     <row r="24" spans="1:32">
-      <c r="M24" s="50"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="50"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="50"/>
-      <c r="T24" s="50"/>
-      <c r="U24" s="50"/>
-      <c r="X24" s="50"/>
-      <c r="Y24" s="50"/>
-      <c r="Z24" s="50"/>
-      <c r="AA24" s="50"/>
-      <c r="AB24" s="50"/>
-      <c r="AC24" s="50"/>
-      <c r="AD24" s="50"/>
-      <c r="AE24" s="50"/>
-      <c r="AF24" s="50"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="40"/>
+      <c r="X24" s="40"/>
+      <c r="Y24" s="40"/>
+      <c r="Z24" s="40"/>
+      <c r="AA24" s="40"/>
+      <c r="AB24" s="40"/>
+      <c r="AC24" s="40"/>
+      <c r="AD24" s="40"/>
+      <c r="AE24" s="40"/>
+      <c r="AF24" s="40"/>
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="25"/>
@@ -2150,96 +2082,96 @@
       <c r="I25" s="24"/>
       <c r="J25" s="24"/>
       <c r="K25" s="26"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="50"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="50"/>
-      <c r="T25" s="50"/>
-      <c r="U25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="50"/>
-      <c r="Z25" s="50"/>
-      <c r="AA25" s="50"/>
-      <c r="AB25" s="50"/>
-      <c r="AC25" s="50"/>
-      <c r="AD25" s="50"/>
-      <c r="AE25" s="50"/>
-      <c r="AF25" s="50"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="40"/>
+      <c r="X25" s="40"/>
+      <c r="Y25" s="40"/>
+      <c r="Z25" s="40"/>
+      <c r="AA25" s="40"/>
+      <c r="AB25" s="40"/>
+      <c r="AC25" s="40"/>
+      <c r="AD25" s="40"/>
+      <c r="AE25" s="40"/>
+      <c r="AF25" s="40"/>
     </row>
     <row r="26" spans="1:32">
-      <c r="M26" s="50"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="50"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="50"/>
-      <c r="R26" s="50"/>
-      <c r="S26" s="50"/>
-      <c r="T26" s="50"/>
-      <c r="U26" s="50"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="50"/>
-      <c r="Z26" s="50"/>
-      <c r="AA26" s="50"/>
-      <c r="AB26" s="50"/>
-      <c r="AC26" s="50"/>
-      <c r="AD26" s="50"/>
-      <c r="AE26" s="50"/>
-      <c r="AF26" s="50"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="40"/>
+      <c r="X26" s="40"/>
+      <c r="Y26" s="40"/>
+      <c r="Z26" s="40"/>
+      <c r="AA26" s="40"/>
+      <c r="AB26" s="40"/>
+      <c r="AC26" s="40"/>
+      <c r="AD26" s="40"/>
+      <c r="AE26" s="40"/>
+      <c r="AF26" s="40"/>
     </row>
     <row r="27" spans="1:32" ht="20.25" customHeight="1">
-      <c r="I27" s="46" t="s">
+      <c r="I27" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="46"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="50"/>
-      <c r="X27" s="50"/>
-      <c r="Y27" s="50"/>
-      <c r="Z27" s="50"/>
-      <c r="AA27" s="50"/>
-      <c r="AB27" s="50"/>
-      <c r="AC27" s="50"/>
-      <c r="AD27" s="50"/>
-      <c r="AE27" s="50"/>
-      <c r="AF27" s="50"/>
-    </row>
-    <row r="28" spans="1:32">
+      <c r="J27" s="38"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="40"/>
+      <c r="X27" s="40"/>
+      <c r="Y27" s="40"/>
+      <c r="Z27" s="40"/>
+      <c r="AA27" s="40"/>
+      <c r="AB27" s="40"/>
+      <c r="AC27" s="40"/>
+      <c r="AD27" s="40"/>
+      <c r="AE27" s="40"/>
+      <c r="AF27" s="40"/>
+    </row>
+    <row r="28" spans="1:32" ht="15">
       <c r="D28" s="45" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E28" s="45"/>
       <c r="F28" s="45"/>
       <c r="G28" s="45"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
-      <c r="T28" s="50"/>
-      <c r="U28" s="50"/>
-      <c r="X28" s="50"/>
-      <c r="Y28" s="50"/>
-      <c r="Z28" s="50"/>
-      <c r="AA28" s="50"/>
-      <c r="AB28" s="50"/>
-      <c r="AC28" s="50"/>
-      <c r="AD28" s="50"/>
-      <c r="AE28" s="50"/>
-      <c r="AF28" s="50"/>
-    </row>
-    <row r="29" spans="1:32">
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="40"/>
+      <c r="U28" s="40"/>
+      <c r="X28" s="40"/>
+      <c r="Y28" s="40"/>
+      <c r="Z28" s="40"/>
+      <c r="AA28" s="40"/>
+      <c r="AB28" s="40"/>
+      <c r="AC28" s="40"/>
+      <c r="AD28" s="40"/>
+      <c r="AE28" s="40"/>
+      <c r="AF28" s="40"/>
+    </row>
+    <row r="29" spans="1:32" ht="15">
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
@@ -2247,61 +2179,55 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
-      <c r="I29" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="50"/>
-      <c r="O29" s="50"/>
-      <c r="P29" s="50"/>
-      <c r="Q29" s="50"/>
-      <c r="R29" s="50"/>
-      <c r="S29" s="50"/>
-      <c r="T29" s="50"/>
-      <c r="U29" s="50"/>
-      <c r="X29" s="50"/>
-      <c r="Y29" s="50"/>
-      <c r="Z29" s="50"/>
-      <c r="AA29" s="50"/>
-      <c r="AB29" s="50"/>
-      <c r="AC29" s="50"/>
-      <c r="AD29" s="50"/>
-      <c r="AE29" s="50"/>
-      <c r="AF29" s="50"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
+      <c r="Z29" s="40"/>
+      <c r="AA29" s="40"/>
+      <c r="AB29" s="40"/>
+      <c r="AC29" s="40"/>
+      <c r="AD29" s="40"/>
+      <c r="AE29" s="40"/>
+      <c r="AF29" s="40"/>
     </row>
     <row r="30" spans="1:32">
       <c r="G30" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30" s="50"/>
-      <c r="N30" s="50"/>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="50"/>
-      <c r="T30" s="50"/>
-      <c r="U30" s="50"/>
-      <c r="X30" s="50"/>
-      <c r="Y30" s="50"/>
-      <c r="Z30" s="50"/>
-      <c r="AA30" s="50"/>
-      <c r="AB30" s="50"/>
-      <c r="AC30" s="50"/>
-      <c r="AD30" s="50"/>
-      <c r="AE30" s="50"/>
-      <c r="AF30" s="50"/>
-    </row>
-    <row r="31" spans="1:32">
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="40"/>
+      <c r="Z30" s="40"/>
+      <c r="AA30" s="40"/>
+      <c r="AB30" s="40"/>
+      <c r="AC30" s="40"/>
+      <c r="AD30" s="40"/>
+      <c r="AE30" s="40"/>
+      <c r="AF30" s="40"/>
+    </row>
+    <row r="31" spans="1:32" ht="15">
       <c r="A31" s="5"/>
       <c r="B31" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -2309,52 +2235,52 @@
       <c r="F31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="50"/>
-      <c r="U31" s="50"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="50"/>
-      <c r="Z31" s="50"/>
-      <c r="AA31" s="50"/>
-      <c r="AB31" s="50"/>
-      <c r="AC31" s="50"/>
-      <c r="AD31" s="50"/>
-      <c r="AE31" s="50"/>
-      <c r="AF31" s="50"/>
-    </row>
-    <row r="32" spans="1:32">
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="X31" s="40"/>
+      <c r="Y31" s="40"/>
+      <c r="Z31" s="40"/>
+      <c r="AA31" s="40"/>
+      <c r="AB31" s="40"/>
+      <c r="AC31" s="40"/>
+      <c r="AD31" s="40"/>
+      <c r="AE31" s="40"/>
+      <c r="AF31" s="40"/>
+    </row>
+    <row r="32" spans="1:32" ht="15">
       <c r="B32" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K32" s="7"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="50"/>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="50"/>
-      <c r="U32" s="50"/>
-      <c r="X32" s="50"/>
-      <c r="Y32" s="50"/>
-      <c r="Z32" s="50"/>
-      <c r="AA32" s="50"/>
-      <c r="AB32" s="50"/>
-      <c r="AC32" s="50"/>
-      <c r="AD32" s="50"/>
-      <c r="AE32" s="50"/>
-      <c r="AF32" s="50"/>
-    </row>
-    <row r="33" spans="1:32">
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="40"/>
+      <c r="X32" s="40"/>
+      <c r="Y32" s="40"/>
+      <c r="Z32" s="40"/>
+      <c r="AA32" s="40"/>
+      <c r="AB32" s="40"/>
+      <c r="AC32" s="40"/>
+      <c r="AD32" s="40"/>
+      <c r="AE32" s="40"/>
+      <c r="AF32" s="40"/>
+    </row>
+    <row r="33" spans="1:32" ht="15">
       <c r="B33" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -2365,112 +2291,100 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="7"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="50"/>
-      <c r="P33" s="50"/>
-      <c r="Q33" s="50"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50"/>
-      <c r="T33" s="50"/>
-      <c r="U33" s="50"/>
-      <c r="X33" s="50"/>
-      <c r="Y33" s="50"/>
-      <c r="Z33" s="50"/>
-      <c r="AA33" s="50"/>
-      <c r="AB33" s="50"/>
-      <c r="AC33" s="50"/>
-      <c r="AD33" s="50"/>
-      <c r="AE33" s="50"/>
-      <c r="AF33" s="50"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="X33" s="40"/>
+      <c r="Y33" s="40"/>
+      <c r="Z33" s="40"/>
+      <c r="AA33" s="40"/>
+      <c r="AB33" s="40"/>
+      <c r="AC33" s="40"/>
+      <c r="AD33" s="40"/>
+      <c r="AE33" s="40"/>
+      <c r="AF33" s="40"/>
     </row>
     <row r="34" spans="1:32" ht="11.25" customHeight="1">
       <c r="A34" s="5"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50"/>
-      <c r="T34" s="50"/>
-      <c r="U34" s="50"/>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="50"/>
-      <c r="Z34" s="50"/>
-      <c r="AA34" s="50"/>
-      <c r="AB34" s="50"/>
-      <c r="AC34" s="50"/>
-      <c r="AD34" s="50"/>
-      <c r="AE34" s="50"/>
-      <c r="AF34" s="50"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="40"/>
+      <c r="U34" s="40"/>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="40"/>
+      <c r="AA34" s="40"/>
+      <c r="AB34" s="40"/>
+      <c r="AC34" s="40"/>
+      <c r="AD34" s="40"/>
+      <c r="AE34" s="40"/>
+      <c r="AF34" s="40"/>
     </row>
     <row r="35" spans="1:32">
       <c r="A35" s="5"/>
       <c r="B35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M35" s="50"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="50"/>
-      <c r="T35" s="50"/>
-      <c r="U35" s="50"/>
-      <c r="X35" s="50"/>
-      <c r="Y35" s="50"/>
-      <c r="Z35" s="50"/>
-      <c r="AA35" s="50"/>
-      <c r="AB35" s="50"/>
-      <c r="AC35" s="50"/>
-      <c r="AD35" s="50"/>
-      <c r="AE35" s="50"/>
-      <c r="AF35" s="50"/>
+      <c r="M35" s="40"/>
+      <c r="N35" s="40"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="40"/>
+      <c r="Q35" s="40"/>
+      <c r="R35" s="40"/>
+      <c r="S35" s="40"/>
+      <c r="T35" s="40"/>
+      <c r="U35" s="40"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
+      <c r="Z35" s="40"/>
+      <c r="AA35" s="40"/>
+      <c r="AB35" s="40"/>
+      <c r="AC35" s="40"/>
+      <c r="AD35" s="40"/>
+      <c r="AE35" s="40"/>
+      <c r="AF35" s="40"/>
     </row>
     <row r="36" spans="1:32">
       <c r="B36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M36" s="50"/>
-      <c r="N36" s="50"/>
-      <c r="O36" s="50"/>
-      <c r="P36" s="50"/>
-      <c r="Q36" s="50"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="50"/>
-      <c r="T36" s="50"/>
-      <c r="U36" s="50"/>
-      <c r="X36" s="50"/>
-      <c r="Y36" s="50"/>
-      <c r="Z36" s="50"/>
-      <c r="AA36" s="50"/>
-      <c r="AB36" s="50"/>
-      <c r="AC36" s="50"/>
-      <c r="AD36" s="50"/>
-      <c r="AE36" s="50"/>
-      <c r="AF36" s="50"/>
-    </row>
-    <row r="37" spans="1:32">
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="40"/>
+      <c r="Q36" s="40"/>
+      <c r="R36" s="40"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="40"/>
+      <c r="X36" s="40"/>
+      <c r="Y36" s="40"/>
+      <c r="Z36" s="40"/>
+      <c r="AA36" s="40"/>
+      <c r="AB36" s="40"/>
+      <c r="AC36" s="40"/>
+      <c r="AD36" s="40"/>
+      <c r="AE36" s="40"/>
+      <c r="AF36" s="40"/>
+    </row>
+    <row r="37" spans="1:32" ht="15">
       <c r="B37" s="14" t="s">
         <v>31</v>
       </c>
@@ -2480,34 +2394,34 @@
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
       <c r="F37" s="19"/>
-      <c r="G37" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="44"/>
+      <c r="G37" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="47"/>
       <c r="I37" s="19" t="s">
         <v>29</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="M37" s="50"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="50"/>
-      <c r="P37" s="50"/>
-      <c r="Q37" s="50"/>
-      <c r="R37" s="50"/>
-      <c r="S37" s="50"/>
-      <c r="T37" s="50"/>
-      <c r="U37" s="50"/>
-      <c r="X37" s="50"/>
-      <c r="Y37" s="50"/>
-      <c r="Z37" s="50"/>
-      <c r="AA37" s="50"/>
-      <c r="AB37" s="50"/>
-      <c r="AC37" s="50"/>
-      <c r="AD37" s="50"/>
-      <c r="AE37" s="50"/>
-      <c r="AF37" s="50"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="40"/>
+      <c r="Q37" s="40"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
+      <c r="T37" s="40"/>
+      <c r="U37" s="40"/>
+      <c r="X37" s="40"/>
+      <c r="Y37" s="40"/>
+      <c r="Z37" s="40"/>
+      <c r="AA37" s="40"/>
+      <c r="AB37" s="40"/>
+      <c r="AC37" s="40"/>
+      <c r="AD37" s="40"/>
+      <c r="AE37" s="40"/>
+      <c r="AF37" s="40"/>
     </row>
     <row r="38" spans="1:32" ht="13.5" customHeight="1">
       <c r="B38" s="15"/>
@@ -2519,24 +2433,24 @@
       <c r="H38" s="35"/>
       <c r="I38" s="35"/>
       <c r="J38" s="28"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="50"/>
-      <c r="S38" s="50"/>
-      <c r="T38" s="50"/>
-      <c r="U38" s="50"/>
-      <c r="X38" s="50"/>
-      <c r="Y38" s="50"/>
-      <c r="Z38" s="50"/>
-      <c r="AA38" s="50"/>
-      <c r="AB38" s="50"/>
-      <c r="AC38" s="50"/>
-      <c r="AD38" s="50"/>
-      <c r="AE38" s="50"/>
-      <c r="AF38" s="50"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="40"/>
+      <c r="R38" s="40"/>
+      <c r="S38" s="40"/>
+      <c r="T38" s="40"/>
+      <c r="U38" s="40"/>
+      <c r="X38" s="40"/>
+      <c r="Y38" s="40"/>
+      <c r="Z38" s="40"/>
+      <c r="AA38" s="40"/>
+      <c r="AB38" s="40"/>
+      <c r="AC38" s="40"/>
+      <c r="AD38" s="40"/>
+      <c r="AE38" s="40"/>
+      <c r="AF38" s="40"/>
     </row>
     <row r="39" spans="1:32" ht="15" customHeight="1">
       <c r="B39" s="15"/>
@@ -2549,25 +2463,25 @@
       <c r="I39" s="35"/>
       <c r="J39" s="28"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="50"/>
-      <c r="R39" s="50"/>
-      <c r="S39" s="50"/>
-      <c r="T39" s="50"/>
-      <c r="U39" s="50"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="40"/>
+      <c r="Q39" s="40"/>
+      <c r="R39" s="40"/>
+      <c r="S39" s="40"/>
+      <c r="T39" s="40"/>
+      <c r="U39" s="40"/>
       <c r="W39" s="2"/>
-      <c r="X39" s="50"/>
-      <c r="Y39" s="50"/>
-      <c r="Z39" s="50"/>
-      <c r="AA39" s="50"/>
-      <c r="AB39" s="50"/>
-      <c r="AC39" s="50"/>
-      <c r="AD39" s="50"/>
-      <c r="AE39" s="50"/>
-      <c r="AF39" s="50"/>
+      <c r="X39" s="40"/>
+      <c r="Y39" s="40"/>
+      <c r="Z39" s="40"/>
+      <c r="AA39" s="40"/>
+      <c r="AB39" s="40"/>
+      <c r="AC39" s="40"/>
+      <c r="AD39" s="40"/>
+      <c r="AE39" s="40"/>
+      <c r="AF39" s="40"/>
     </row>
     <row r="40" spans="1:32" ht="14.25" customHeight="1">
       <c r="B40" s="15"/>
@@ -2579,26 +2493,26 @@
       <c r="H40" s="35"/>
       <c r="I40" s="35"/>
       <c r="J40" s="28"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="50"/>
-      <c r="R40" s="50"/>
-      <c r="S40" s="50"/>
-      <c r="T40" s="50"/>
-      <c r="U40" s="50"/>
-      <c r="X40" s="50"/>
-      <c r="Y40" s="50"/>
-      <c r="Z40" s="50"/>
-      <c r="AA40" s="50"/>
-      <c r="AB40" s="50"/>
-      <c r="AC40" s="50"/>
-      <c r="AD40" s="50"/>
-      <c r="AE40" s="50"/>
-      <c r="AF40" s="50"/>
-    </row>
-    <row r="41" spans="1:32">
+      <c r="M40" s="40"/>
+      <c r="N40" s="40"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="40"/>
+      <c r="R40" s="40"/>
+      <c r="S40" s="40"/>
+      <c r="T40" s="40"/>
+      <c r="U40" s="40"/>
+      <c r="X40" s="40"/>
+      <c r="Y40" s="40"/>
+      <c r="Z40" s="40"/>
+      <c r="AA40" s="40"/>
+      <c r="AB40" s="40"/>
+      <c r="AC40" s="40"/>
+      <c r="AD40" s="40"/>
+      <c r="AE40" s="40"/>
+      <c r="AF40" s="40"/>
+    </row>
+    <row r="41" spans="1:32" ht="15">
       <c r="B41" s="15"/>
       <c r="C41" s="16"/>
       <c r="D41" s="17"/>
@@ -2608,26 +2522,26 @@
       <c r="H41" s="35"/>
       <c r="I41" s="35"/>
       <c r="J41" s="28"/>
-      <c r="M41" s="50"/>
-      <c r="N41" s="50"/>
-      <c r="O41" s="50"/>
-      <c r="P41" s="50"/>
-      <c r="Q41" s="50"/>
-      <c r="R41" s="50"/>
-      <c r="S41" s="50"/>
-      <c r="T41" s="50"/>
-      <c r="U41" s="50"/>
-      <c r="X41" s="50"/>
-      <c r="Y41" s="50"/>
-      <c r="Z41" s="50"/>
-      <c r="AA41" s="50"/>
-      <c r="AB41" s="50"/>
-      <c r="AC41" s="50"/>
-      <c r="AD41" s="50"/>
-      <c r="AE41" s="50"/>
-      <c r="AF41" s="50"/>
-    </row>
-    <row r="42" spans="1:32">
+      <c r="M41" s="40"/>
+      <c r="N41" s="40"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+      <c r="T41" s="40"/>
+      <c r="U41" s="40"/>
+      <c r="X41" s="40"/>
+      <c r="Y41" s="40"/>
+      <c r="Z41" s="40"/>
+      <c r="AA41" s="40"/>
+      <c r="AB41" s="40"/>
+      <c r="AC41" s="40"/>
+      <c r="AD41" s="40"/>
+      <c r="AE41" s="40"/>
+      <c r="AF41" s="40"/>
+    </row>
+    <row r="42" spans="1:32" ht="15">
       <c r="B42" s="15"/>
       <c r="C42" s="16"/>
       <c r="D42" s="17"/>
@@ -2637,146 +2551,137 @@
       <c r="H42" s="37"/>
       <c r="I42" s="35"/>
       <c r="J42" s="28"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="50"/>
-      <c r="S42" s="50"/>
-      <c r="T42" s="50"/>
-      <c r="U42" s="50"/>
-      <c r="X42" s="50"/>
-      <c r="Y42" s="50"/>
-      <c r="Z42" s="50"/>
-      <c r="AA42" s="50"/>
-      <c r="AB42" s="50"/>
-      <c r="AC42" s="50"/>
-      <c r="AD42" s="50"/>
-      <c r="AE42" s="50"/>
-      <c r="AF42" s="50"/>
-    </row>
-    <row r="43" spans="1:32">
-      <c r="B43" s="38" t="s">
+      <c r="M42" s="40"/>
+      <c r="N42" s="40"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="40"/>
+      <c r="Q42" s="40"/>
+      <c r="R42" s="40"/>
+      <c r="S42" s="40"/>
+      <c r="T42" s="40"/>
+      <c r="U42" s="40"/>
+      <c r="X42" s="40"/>
+      <c r="Y42" s="40"/>
+      <c r="Z42" s="40"/>
+      <c r="AA42" s="40"/>
+      <c r="AB42" s="40"/>
+      <c r="AC42" s="40"/>
+      <c r="AD42" s="40"/>
+      <c r="AE42" s="40"/>
+      <c r="AF42" s="40"/>
+    </row>
+    <row r="43" spans="1:32" ht="15">
+      <c r="B43" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="39"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="50"/>
       <c r="J43" s="29"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="50"/>
-      <c r="R43" s="50"/>
-      <c r="S43" s="50"/>
-      <c r="T43" s="50"/>
-      <c r="U43" s="50"/>
-      <c r="X43" s="50"/>
-      <c r="Y43" s="50"/>
-      <c r="Z43" s="50"/>
-      <c r="AA43" s="50"/>
-      <c r="AB43" s="50"/>
-      <c r="AC43" s="50"/>
-      <c r="AD43" s="50"/>
-      <c r="AE43" s="50"/>
-      <c r="AF43" s="50"/>
-    </row>
-    <row r="44" spans="1:32">
+      <c r="M43" s="40"/>
+      <c r="N43" s="40"/>
+      <c r="O43" s="40"/>
+      <c r="P43" s="40"/>
+      <c r="Q43" s="40"/>
+      <c r="R43" s="40"/>
+      <c r="S43" s="40"/>
+      <c r="T43" s="40"/>
+      <c r="U43" s="40"/>
+      <c r="X43" s="40"/>
+      <c r="Y43" s="40"/>
+      <c r="Z43" s="40"/>
+      <c r="AA43" s="40"/>
+      <c r="AB43" s="40"/>
+      <c r="AC43" s="40"/>
+      <c r="AD43" s="40"/>
+      <c r="AE43" s="40"/>
+      <c r="AF43" s="40"/>
+    </row>
+    <row r="44" spans="1:32" ht="15">
       <c r="B44" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
-      <c r="H44" s="38" t="s">
+      <c r="H44" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="I44" s="39"/>
+      <c r="I44" s="50"/>
       <c r="J44" s="30">
         <f>SUM(J38:J43)</f>
         <v>0</v>
       </c>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50"/>
-      <c r="R44" s="50"/>
-      <c r="S44" s="50"/>
-      <c r="T44" s="50"/>
-      <c r="U44" s="50"/>
-      <c r="X44" s="50"/>
-      <c r="Y44" s="50"/>
-      <c r="Z44" s="50"/>
-      <c r="AA44" s="50"/>
-      <c r="AB44" s="50"/>
-      <c r="AC44" s="50"/>
-      <c r="AD44" s="50"/>
-      <c r="AE44" s="50"/>
-      <c r="AF44" s="50"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="40"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="40"/>
+      <c r="R44" s="40"/>
+      <c r="S44" s="40"/>
+      <c r="T44" s="40"/>
+      <c r="U44" s="40"/>
+      <c r="X44" s="40"/>
+      <c r="Y44" s="40"/>
+      <c r="Z44" s="40"/>
+      <c r="AA44" s="40"/>
+      <c r="AB44" s="40"/>
+      <c r="AC44" s="40"/>
+      <c r="AD44" s="40"/>
+      <c r="AE44" s="40"/>
+      <c r="AF44" s="40"/>
     </row>
     <row r="45" spans="1:32">
       <c r="B45" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="M45" s="50"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="50"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="50"/>
-      <c r="R45" s="50"/>
-      <c r="S45" s="50"/>
-      <c r="T45" s="50"/>
-      <c r="U45" s="50"/>
-      <c r="X45" s="50"/>
-      <c r="Y45" s="50"/>
-      <c r="Z45" s="50"/>
-      <c r="AA45" s="50"/>
-      <c r="AB45" s="50"/>
-      <c r="AC45" s="50"/>
-      <c r="AD45" s="50"/>
-      <c r="AE45" s="50"/>
-      <c r="AF45" s="50"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="40"/>
+      <c r="O45" s="40"/>
+      <c r="P45" s="40"/>
+      <c r="Q45" s="40"/>
+      <c r="R45" s="40"/>
+      <c r="S45" s="40"/>
+      <c r="T45" s="40"/>
+      <c r="U45" s="40"/>
+      <c r="X45" s="40"/>
+      <c r="Y45" s="40"/>
+      <c r="Z45" s="40"/>
+      <c r="AA45" s="40"/>
+      <c r="AB45" s="40"/>
+      <c r="AC45" s="40"/>
+      <c r="AD45" s="40"/>
+      <c r="AE45" s="40"/>
+      <c r="AF45" s="40"/>
     </row>
     <row r="46" spans="1:32">
       <c r="J46" s="23"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="50"/>
-      <c r="O46" s="50"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="50"/>
-      <c r="R46" s="50"/>
-      <c r="S46" s="50"/>
-      <c r="T46" s="50"/>
-      <c r="U46" s="50"/>
-      <c r="X46" s="50"/>
-      <c r="Y46" s="50"/>
-      <c r="Z46" s="50"/>
-      <c r="AA46" s="50"/>
-      <c r="AB46" s="50"/>
-      <c r="AC46" s="50"/>
-      <c r="AD46" s="50"/>
-      <c r="AE46" s="50"/>
-      <c r="AF46" s="50"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="40"/>
+      <c r="O46" s="40"/>
+      <c r="P46" s="40"/>
+      <c r="Q46" s="40"/>
+      <c r="R46" s="40"/>
+      <c r="S46" s="40"/>
+      <c r="T46" s="40"/>
+      <c r="U46" s="40"/>
+      <c r="X46" s="40"/>
+      <c r="Y46" s="40"/>
+      <c r="Z46" s="40"/>
+      <c r="AA46" s="40"/>
+      <c r="AB46" s="40"/>
+      <c r="AC46" s="40"/>
+      <c r="AD46" s="40"/>
+      <c r="AE46" s="40"/>
+      <c r="AF46" s="40"/>
     </row>
     <row r="47" spans="1:32">
       <c r="B47" s="24"/>
@@ -2790,52 +2695,52 @@
       <c r="J47" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M47" s="50"/>
-      <c r="N47" s="50"/>
-      <c r="O47" s="50"/>
-      <c r="P47" s="50"/>
-      <c r="Q47" s="50"/>
-      <c r="R47" s="50"/>
-      <c r="S47" s="50"/>
-      <c r="T47" s="50"/>
-      <c r="U47" s="50"/>
-      <c r="X47" s="50"/>
-      <c r="Y47" s="50"/>
-      <c r="Z47" s="50"/>
-      <c r="AA47" s="50"/>
-      <c r="AB47" s="50"/>
-      <c r="AC47" s="50"/>
-      <c r="AD47" s="50"/>
-      <c r="AE47" s="50"/>
-      <c r="AF47" s="50"/>
+      <c r="M47" s="40"/>
+      <c r="N47" s="40"/>
+      <c r="O47" s="40"/>
+      <c r="P47" s="40"/>
+      <c r="Q47" s="40"/>
+      <c r="R47" s="40"/>
+      <c r="S47" s="40"/>
+      <c r="T47" s="40"/>
+      <c r="U47" s="40"/>
+      <c r="X47" s="40"/>
+      <c r="Y47" s="40"/>
+      <c r="Z47" s="40"/>
+      <c r="AA47" s="40"/>
+      <c r="AB47" s="40"/>
+      <c r="AC47" s="40"/>
+      <c r="AD47" s="40"/>
+      <c r="AE47" s="40"/>
+      <c r="AF47" s="40"/>
     </row>
     <row r="49" spans="2:32" ht="22.5" customHeight="1">
-      <c r="M49" s="49" t="s">
+      <c r="M49" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="N49" s="49"/>
-      <c r="O49" s="49"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="39"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
-      <c r="R49" s="49" t="s">
+      <c r="R49" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="S49" s="49"/>
-      <c r="T49" s="49"/>
-      <c r="U49" s="49"/>
-      <c r="X49" s="49" t="s">
+      <c r="S49" s="39"/>
+      <c r="T49" s="39"/>
+      <c r="U49" s="39"/>
+      <c r="X49" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="Y49" s="49"/>
-      <c r="Z49" s="49"/>
+      <c r="Y49" s="39"/>
+      <c r="Z49" s="39"/>
       <c r="AA49" s="11"/>
       <c r="AB49" s="11"/>
-      <c r="AC49" s="49" t="s">
+      <c r="AC49" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="AD49" s="49"/>
-      <c r="AE49" s="49"/>
-      <c r="AF49" s="49"/>
+      <c r="AD49" s="39"/>
+      <c r="AE49" s="39"/>
+      <c r="AF49" s="39"/>
     </row>
     <row r="50" spans="2:32">
       <c r="M50" s="11"/>
@@ -2944,6 +2849,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="L6:V6"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="L7:V7"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="X49:Z49"/>
     <mergeCell ref="AC49:AF49"/>
@@ -2958,19 +2874,8 @@
     <mergeCell ref="X19:AF47"/>
     <mergeCell ref="L8:V8"/>
     <mergeCell ref="T2:U2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="G6:H6"/>
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="L4:V4"/>
-    <mergeCell ref="L6:V6"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="L7:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>